<commit_message>
check on other test scenarios
</commit_message>
<xml_diff>
--- a/test/validationdata/allscenarios.xlsx
+++ b/test/validationdata/allscenarios.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\risingj\Dropbox\NextGen IAMs\PAGE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23190" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26260" windowHeight="15640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,8 +75,11 @@
     <definedName name="te_a">[1]Totals!$L$12</definedName>
     <definedName name="WORLDB_GDPPOP_SWITCH">[1]Cockpit!$B$54</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -90,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="37">
   <si>
     <t>RF A</t>
   </si>
@@ -202,18 +200,6 @@
   <si>
     <t>Nonlinear PCF &amp; SAF</t>
   </si>
-  <si>
-    <t>SCCO2 Nonlinear PCF</t>
-  </si>
-  <si>
-    <t>SCCO2 Nonlinear SAF</t>
-  </si>
-  <si>
-    <t>SCCO2 Nonlinear PCF &amp; SAF</t>
-  </si>
-  <si>
-    <t>SCCO2 Legacy PCF &amp; SAF</t>
-  </si>
 </sst>
 </file>
 
@@ -222,7 +208,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +226,22 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -265,8 +267,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -286,7 +294,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -303,7 +317,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Readme"/>
@@ -427,7 +441,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -462,7 +476,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -639,7 +653,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -647,18 +661,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI33"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -738,25 +752,19 @@
         <v>36</v>
       </c>
       <c r="AB1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AC1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AD1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AE1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF1" t="s">
         <v>36</v>
       </c>
-      <c r="AH1" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -836,25 +844,19 @@
         <v>29</v>
       </c>
       <c r="AB2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="AC2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="AD2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="AE2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -940,25 +942,13 @@
         <v>6</v>
       </c>
       <c r="AD3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="AE3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH3" t="s">
         <v>22</v>
       </c>
-      <c r="AI3" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -1049,20 +1039,8 @@
       <c r="AE4" t="s">
         <v>7</v>
       </c>
-      <c r="AF4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -1145,28 +1123,16 @@
         <v>19</v>
       </c>
       <c r="AC5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AD5" t="s">
         <v>19</v>
       </c>
       <c r="AE5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG5" t="s">
         <v>20</v>
       </c>
-      <c r="AH5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -1260,20 +1226,8 @@
       <c r="AE6" t="s">
         <v>0</v>
       </c>
-      <c r="AF6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1356,31 +1310,19 @@
         <v>5.1480453778884785</v>
       </c>
       <c r="AB7">
-        <v>4.9987772417132321</v>
+        <v>2.9040624640793529</v>
       </c>
       <c r="AC7">
-        <v>5.1478905438868807</v>
+        <v>2.4992024116663876</v>
       </c>
       <c r="AD7">
-        <v>4.9988298912005087</v>
+        <v>8.333851990978463</v>
       </c>
       <c r="AE7">
-        <v>5.1480453778884785</v>
-      </c>
-      <c r="AF7">
-        <v>2.9040624640793529</v>
-      </c>
-      <c r="AG7">
-        <v>2.4992024116663876</v>
-      </c>
-      <c r="AH7">
-        <v>8.333851990978463</v>
-      </c>
-      <c r="AI7">
         <v>7.6392820268130155</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -1463,31 +1405,19 @@
         <v>5.1480453778884785</v>
       </c>
       <c r="AB8">
-        <v>4.9987772417132321</v>
+        <v>2.9040624640793529</v>
       </c>
       <c r="AC8">
-        <v>5.1478905438868807</v>
+        <v>2.7394590039709823</v>
       </c>
       <c r="AD8">
-        <v>4.9988298912005087</v>
+        <v>8.333851990978463</v>
       </c>
       <c r="AE8">
-        <v>5.1480453778884785</v>
-      </c>
-      <c r="AF8">
-        <v>2.9040624640793529</v>
-      </c>
-      <c r="AG8">
-        <v>2.7394590039709823</v>
-      </c>
-      <c r="AH8">
-        <v>8.333851990978463</v>
-      </c>
-      <c r="AI8">
         <v>8.0659342945618775</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
@@ -1570,31 +1500,19 @@
         <v>5.1480453778884785</v>
       </c>
       <c r="AB9">
-        <v>4.9987772417132321</v>
+        <v>2.9040624640793529</v>
       </c>
       <c r="AC9">
-        <v>5.1478905438868807</v>
+        <v>2.9143387416384865</v>
       </c>
       <c r="AD9">
-        <v>4.9988298912005087</v>
+        <v>8.333851990978463</v>
       </c>
       <c r="AE9">
-        <v>5.1480453778884785</v>
-      </c>
-      <c r="AF9">
-        <v>2.9040624640793529</v>
-      </c>
-      <c r="AG9">
-        <v>2.9143387416384865</v>
-      </c>
-      <c r="AH9">
-        <v>8.333851990978463</v>
-      </c>
-      <c r="AI9">
         <v>8.3311554994728017</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31">
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
@@ -1677,31 +1595,19 @@
         <v>5.1480453778884785</v>
       </c>
       <c r="AB10">
-        <v>4.9987772417132321</v>
+        <v>2.9040624640793529</v>
       </c>
       <c r="AC10">
-        <v>5.1478905438868807</v>
+        <v>3.0695023535622896</v>
       </c>
       <c r="AD10">
-        <v>4.9988298912005087</v>
+        <v>8.333851990978463</v>
       </c>
       <c r="AE10">
-        <v>5.1480453778884785</v>
-      </c>
-      <c r="AF10">
-        <v>2.9040624640793529</v>
-      </c>
-      <c r="AG10">
-        <v>3.0695023535622896</v>
-      </c>
-      <c r="AH10">
-        <v>8.333851990978463</v>
-      </c>
-      <c r="AI10">
         <v>8.592040371057287</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -1784,31 +1690,19 @@
         <v>5.1480453778884785</v>
       </c>
       <c r="AB11">
-        <v>4.9987772417132321</v>
+        <v>2.9040624640793529</v>
       </c>
       <c r="AC11">
-        <v>5.1478905438868807</v>
+        <v>3.2650526964623374</v>
       </c>
       <c r="AD11">
-        <v>4.9988298912005087</v>
+        <v>8.333851990978463</v>
       </c>
       <c r="AE11">
-        <v>5.1480453778884785</v>
-      </c>
-      <c r="AF11">
-        <v>2.9040624640793529</v>
-      </c>
-      <c r="AG11">
-        <v>3.2650526964623374</v>
-      </c>
-      <c r="AH11">
-        <v>8.333851990978463</v>
-      </c>
-      <c r="AI11">
         <v>8.9033056335636278</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31">
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
@@ -1891,31 +1785,19 @@
         <v>5.1480453778884785</v>
       </c>
       <c r="AB12">
-        <v>4.9987772417132321</v>
+        <v>2.9040624640793529</v>
       </c>
       <c r="AC12">
-        <v>5.1478905438868807</v>
+        <v>2.9017230824000313</v>
       </c>
       <c r="AD12">
-        <v>4.9988298912005087</v>
+        <v>8.333851990978463</v>
       </c>
       <c r="AE12">
-        <v>5.1480453778884785</v>
-      </c>
-      <c r="AF12">
-        <v>2.9040624640793529</v>
-      </c>
-      <c r="AG12">
-        <v>2.9017230824000313</v>
-      </c>
-      <c r="AH12">
-        <v>8.333851990978463</v>
-      </c>
-      <c r="AI12">
         <v>8.3164763676177778</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -2009,20 +1891,8 @@
       <c r="AE13" t="s">
         <v>1</v>
       </c>
-      <c r="AF13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -2105,31 +1975,19 @@
         <v>3.4029035648430739</v>
       </c>
       <c r="AB14">
-        <v>3.3265564443101328</v>
+        <v>2.2089938603464621</v>
       </c>
       <c r="AC14">
-        <v>3.4054240833344198</v>
+        <v>1.2678368438223693</v>
       </c>
       <c r="AD14">
-        <v>3.3247280951413267</v>
+        <v>4.9186692715684615</v>
       </c>
       <c r="AE14">
-        <v>3.4029035648430739</v>
-      </c>
-      <c r="AF14">
-        <v>2.2089938603464621</v>
-      </c>
-      <c r="AG14">
-        <v>1.2678368438223693</v>
-      </c>
-      <c r="AH14">
-        <v>4.9186692715684615</v>
-      </c>
-      <c r="AI14">
         <v>2.9653073803573937</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31">
       <c r="A15" s="7" t="s">
         <v>10</v>
       </c>
@@ -2212,31 +2070,19 @@
         <v>3.4029035648430739</v>
       </c>
       <c r="AB15">
-        <v>3.3265564443101328</v>
+        <v>2.2089938603464621</v>
       </c>
       <c r="AC15">
-        <v>3.4054240833344198</v>
+        <v>1.7710945159304599</v>
       </c>
       <c r="AD15">
-        <v>3.3247280951413267</v>
+        <v>4.9186692715684615</v>
       </c>
       <c r="AE15">
-        <v>3.4029035648430739</v>
-      </c>
-      <c r="AF15">
-        <v>2.2089938603464621</v>
-      </c>
-      <c r="AG15">
-        <v>1.7710945159304599</v>
-      </c>
-      <c r="AH15">
-        <v>4.9186692715684615</v>
-      </c>
-      <c r="AI15">
         <v>4.022442023481922</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31">
       <c r="A16" s="7" t="s">
         <v>11</v>
       </c>
@@ -2319,31 +2165,19 @@
         <v>3.4029035648430739</v>
       </c>
       <c r="AB16">
-        <v>3.3265564443101328</v>
+        <v>2.2089938603464621</v>
       </c>
       <c r="AC16">
-        <v>3.4054240833344198</v>
+        <v>2.146883850511522</v>
       </c>
       <c r="AD16">
-        <v>3.3247280951413267</v>
+        <v>4.9186692715684615</v>
       </c>
       <c r="AE16">
-        <v>3.4029035648430739</v>
-      </c>
-      <c r="AF16">
-        <v>2.2089938603464621</v>
-      </c>
-      <c r="AG16">
-        <v>2.146883850511522</v>
-      </c>
-      <c r="AH16">
-        <v>4.9186692715684615</v>
-      </c>
-      <c r="AI16">
         <v>4.8480538209796968</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31">
       <c r="A17" s="7" t="s">
         <v>12</v>
       </c>
@@ -2426,31 +2260,19 @@
         <v>3.4029035648430739</v>
       </c>
       <c r="AB17">
-        <v>3.3265564443101328</v>
+        <v>2.2089938603464621</v>
       </c>
       <c r="AC17">
-        <v>3.4054240833344198</v>
+        <v>2.5899317093726739</v>
       </c>
       <c r="AD17">
-        <v>3.3247280951413267</v>
+        <v>4.9186692715684615</v>
       </c>
       <c r="AE17">
-        <v>3.4029035648430739</v>
-      </c>
-      <c r="AF17">
-        <v>2.2089938603464621</v>
-      </c>
-      <c r="AG17">
-        <v>2.5899317093726739</v>
-      </c>
-      <c r="AH17">
-        <v>4.9186692715684615</v>
-      </c>
-      <c r="AI17">
         <v>5.7409995706266859</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31">
       <c r="A18" s="7" t="s">
         <v>13</v>
       </c>
@@ -2533,31 +2355,19 @@
         <v>3.4029035648430739</v>
       </c>
       <c r="AB18">
-        <v>3.3265564443101328</v>
+        <v>2.2089938603464621</v>
       </c>
       <c r="AC18">
-        <v>3.4054240833344198</v>
+        <v>3.1873888807270898</v>
       </c>
       <c r="AD18">
-        <v>3.3247280951413267</v>
+        <v>4.9186692715684615</v>
       </c>
       <c r="AE18">
-        <v>3.4029035648430739</v>
-      </c>
-      <c r="AF18">
-        <v>2.2089938603464621</v>
-      </c>
-      <c r="AG18">
-        <v>3.1873888807270898</v>
-      </c>
-      <c r="AH18">
-        <v>4.9186692715684615</v>
-      </c>
-      <c r="AI18">
         <v>6.862233075305781</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31">
       <c r="A19" s="7" t="s">
         <v>14</v>
       </c>
@@ -2640,31 +2450,19 @@
         <v>3.4029035648430739</v>
       </c>
       <c r="AB19">
-        <v>3.3265564443101328</v>
+        <v>2.2089938603464621</v>
       </c>
       <c r="AC19">
-        <v>3.4054240833344198</v>
+        <v>2.191720111000226</v>
       </c>
       <c r="AD19">
-        <v>3.3247280951413267</v>
+        <v>4.9186692715684615</v>
       </c>
       <c r="AE19">
-        <v>3.4029035648430739</v>
-      </c>
-      <c r="AF19">
-        <v>2.2089938603464621</v>
-      </c>
-      <c r="AG19">
-        <v>2.191720111000226</v>
-      </c>
-      <c r="AH19">
-        <v>4.9186692715684615</v>
-      </c>
-      <c r="AI19">
         <v>4.8943847152737208</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31">
       <c r="A20" s="6" t="s">
         <v>16</v>
       </c>
@@ -2758,20 +2556,8 @@
       <c r="AE20" t="s">
         <v>2</v>
       </c>
-      <c r="AF20" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31">
       <c r="A21" s="7" t="s">
         <v>9</v>
       </c>
@@ -2854,31 +2640,19 @@
         <v>1.2481026764606209</v>
       </c>
       <c r="AB21">
-        <v>1.2325795173338541</v>
+        <v>1.0363097502314751</v>
       </c>
       <c r="AC21">
-        <v>1.2474740673804752</v>
+        <v>0.64123489238498621</v>
       </c>
       <c r="AD21">
-        <v>1.2332960360207679</v>
+        <v>1.5004758493226762</v>
       </c>
       <c r="AE21">
-        <v>1.2481026764606209</v>
-      </c>
-      <c r="AF21">
-        <v>1.0363097502314751</v>
-      </c>
-      <c r="AG21">
-        <v>0.64123489238498621</v>
-      </c>
-      <c r="AH21">
-        <v>1.5004758493226762</v>
-      </c>
-      <c r="AI21">
         <v>0.89277030781300215</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31">
       <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
@@ -2961,31 +2735,19 @@
         <v>1.2481026764606209</v>
       </c>
       <c r="AB22">
-        <v>1.2325795173338541</v>
+        <v>1.0363097502314751</v>
       </c>
       <c r="AC22">
-        <v>1.2474740673804752</v>
+        <v>0.83949296384721794</v>
       </c>
       <c r="AD22">
-        <v>1.2332960360207679</v>
+        <v>1.5004758493226762</v>
       </c>
       <c r="AE22">
-        <v>1.2481026764606209</v>
-      </c>
-      <c r="AF22">
-        <v>1.0363097502314751</v>
-      </c>
-      <c r="AG22">
-        <v>0.83949296384721794</v>
-      </c>
-      <c r="AH22">
-        <v>1.5004758493226762</v>
-      </c>
-      <c r="AI22">
         <v>1.1572125202103718</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31">
       <c r="A23" s="7" t="s">
         <v>11</v>
       </c>
@@ -3068,31 +2830,19 @@
         <v>1.2481026764606209</v>
       </c>
       <c r="AB23">
-        <v>1.2325795173338541</v>
+        <v>1.0363097502314751</v>
       </c>
       <c r="AC23">
-        <v>1.2474740673804752</v>
+        <v>1.0150952113927332</v>
       </c>
       <c r="AD23">
-        <v>1.2332960360207679</v>
+        <v>1.5004758493226762</v>
       </c>
       <c r="AE23">
-        <v>1.2481026764606209</v>
-      </c>
-      <c r="AF23">
-        <v>1.0363097502314751</v>
-      </c>
-      <c r="AG23">
-        <v>1.0150952113927332</v>
-      </c>
-      <c r="AH23">
-        <v>1.5004758493226762</v>
-      </c>
-      <c r="AI23">
         <v>1.4754790604121841</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31">
       <c r="A24" s="7" t="s">
         <v>12</v>
       </c>
@@ -3175,31 +2925,19 @@
         <v>1.2481026764606209</v>
       </c>
       <c r="AB24">
-        <v>1.2325795173338541</v>
+        <v>1.0363097502314751</v>
       </c>
       <c r="AC24">
-        <v>1.2474740673804752</v>
+        <v>1.2338932275504071</v>
       </c>
       <c r="AD24">
-        <v>1.2332960360207679</v>
+        <v>1.5004758493226762</v>
       </c>
       <c r="AE24">
-        <v>1.2481026764606209</v>
-      </c>
-      <c r="AF24">
-        <v>1.0363097502314751</v>
-      </c>
-      <c r="AG24">
-        <v>1.2338932275504071</v>
-      </c>
-      <c r="AH24">
-        <v>1.5004758493226762</v>
-      </c>
-      <c r="AI24">
         <v>1.8549626061858024</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31">
       <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
@@ -3282,31 +3020,19 @@
         <v>1.2481026764606209</v>
       </c>
       <c r="AB25">
-        <v>1.2325795173338541</v>
+        <v>1.0363097502314751</v>
       </c>
       <c r="AC25">
-        <v>1.2474740673804752</v>
+        <v>1.6702748988013891</v>
       </c>
       <c r="AD25">
-        <v>1.2332960360207679</v>
+        <v>1.5004758493226762</v>
       </c>
       <c r="AE25">
-        <v>1.2481026764606209</v>
-      </c>
-      <c r="AF25">
-        <v>1.0363097502314751</v>
-      </c>
-      <c r="AG25">
-        <v>1.6702748988013891</v>
-      </c>
-      <c r="AH25">
-        <v>1.5004758493226762</v>
-      </c>
-      <c r="AI25">
         <v>2.6279710227998683</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31">
       <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
@@ -3389,31 +3115,19 @@
         <v>1.2481026764606209</v>
       </c>
       <c r="AB26">
-        <v>1.2325795173338541</v>
+        <v>1.0363097502314751</v>
       </c>
       <c r="AC26">
-        <v>1.2474740673804752</v>
+        <v>1.0737362209686903</v>
       </c>
       <c r="AD26">
-        <v>1.2332960360207679</v>
+        <v>1.5004758493226762</v>
       </c>
       <c r="AE26">
-        <v>1.2481026764606209</v>
-      </c>
-      <c r="AF26">
-        <v>1.0363097502314751</v>
-      </c>
-      <c r="AG26">
-        <v>1.0737362209686903</v>
-      </c>
-      <c r="AH26">
-        <v>1.5004758493226762</v>
-      </c>
-      <c r="AI26">
         <v>1.5657695066202073</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31">
       <c r="A27" s="6" t="s">
         <v>17</v>
       </c>
@@ -3507,20 +3221,8 @@
       <c r="AE27" t="s">
         <v>3</v>
       </c>
-      <c r="AF27" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI27" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31">
       <c r="A28" s="7" t="s">
         <v>9</v>
       </c>
@@ -3603,31 +3305,19 @@
         <v>1027.843539311232</v>
       </c>
       <c r="AB28">
-        <v>946.21797580120085</v>
+        <v>509.0746984757775</v>
       </c>
       <c r="AC28">
-        <v>1032.0923880568128</v>
+        <v>275.42025307261019</v>
       </c>
       <c r="AD28">
-        <v>943.0116782943511</v>
+        <v>1266.418152249259</v>
       </c>
       <c r="AE28">
-        <v>1027.843539311232</v>
-      </c>
-      <c r="AF28">
-        <v>509.0746984757775</v>
-      </c>
-      <c r="AG28">
-        <v>275.42025307261019</v>
-      </c>
-      <c r="AH28">
-        <v>1266.418152249259</v>
-      </c>
-      <c r="AI28">
         <v>276.27384529273735</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31">
       <c r="A29" s="7" t="s">
         <v>10</v>
       </c>
@@ -3710,31 +3400,19 @@
         <v>1027.843539311232</v>
       </c>
       <c r="AB29">
-        <v>946.21797580120085</v>
+        <v>509.0746984757775</v>
       </c>
       <c r="AC29">
-        <v>1032.0923880568128</v>
+        <v>420.12101513960937</v>
       </c>
       <c r="AD29">
-        <v>943.0116782943511</v>
+        <v>1266.418152249259</v>
       </c>
       <c r="AE29">
-        <v>1027.843539311232</v>
-      </c>
-      <c r="AF29">
-        <v>509.0746984757775</v>
-      </c>
-      <c r="AG29">
-        <v>420.12101513960937</v>
-      </c>
-      <c r="AH29">
-        <v>1266.418152249259</v>
-      </c>
-      <c r="AI29">
         <v>709.59969527234648</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31">
       <c r="A30" s="7" t="s">
         <v>11</v>
       </c>
@@ -3817,31 +3495,19 @@
         <v>1027.843539311232</v>
       </c>
       <c r="AB30">
-        <v>946.21797580120085</v>
+        <v>509.0746984757775</v>
       </c>
       <c r="AC30">
-        <v>1032.0923880568128</v>
+        <v>562.99137924235811</v>
       </c>
       <c r="AD30">
-        <v>943.0116782943511</v>
+        <v>1266.418152249259</v>
       </c>
       <c r="AE30">
-        <v>1027.843539311232</v>
-      </c>
-      <c r="AF30">
-        <v>509.0746984757775</v>
-      </c>
-      <c r="AG30">
-        <v>562.99137924235811</v>
-      </c>
-      <c r="AH30">
-        <v>1266.418152249259</v>
-      </c>
-      <c r="AI30">
         <v>1328.3732490802738</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31">
       <c r="A31" s="7" t="s">
         <v>12</v>
       </c>
@@ -3924,31 +3590,19 @@
         <v>1027.843539311232</v>
       </c>
       <c r="AB31">
-        <v>946.21797580120085</v>
+        <v>509.0746984757775</v>
       </c>
       <c r="AC31">
-        <v>1032.0923880568128</v>
+        <v>762.61175222332395</v>
       </c>
       <c r="AD31">
-        <v>943.0116782943511</v>
+        <v>1266.418152249259</v>
       </c>
       <c r="AE31">
-        <v>1027.843539311232</v>
-      </c>
-      <c r="AF31">
-        <v>509.0746984757775</v>
-      </c>
-      <c r="AG31">
-        <v>762.61175222332395</v>
-      </c>
-      <c r="AH31">
-        <v>1266.418152249259</v>
-      </c>
-      <c r="AI31">
         <v>2737.1570634125933</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31">
       <c r="A32" s="7" t="s">
         <v>13</v>
       </c>
@@ -4031,31 +3685,19 @@
         <v>1027.843539311232</v>
       </c>
       <c r="AB32">
-        <v>946.21797580120085</v>
+        <v>509.0746984757775</v>
       </c>
       <c r="AC32">
-        <v>1032.0923880568128</v>
+        <v>1186.5228254425197</v>
       </c>
       <c r="AD32">
-        <v>943.0116782943511</v>
+        <v>1266.418152249259</v>
       </c>
       <c r="AE32">
-        <v>1027.843539311232</v>
-      </c>
-      <c r="AF32">
-        <v>509.0746984757775</v>
-      </c>
-      <c r="AG32">
-        <v>1186.5228254425197</v>
-      </c>
-      <c r="AH32">
-        <v>1266.418152249259</v>
-      </c>
-      <c r="AI32">
         <v>8653.3151521333057</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31">
       <c r="A33" s="7" t="s">
         <v>14</v>
       </c>
@@ -4138,31 +3780,25 @@
         <v>1027.843539311232</v>
       </c>
       <c r="AB33">
-        <v>946.21797580120085</v>
+        <v>509.0746984757775</v>
       </c>
       <c r="AC33">
-        <v>1032.0923880568128</v>
+        <v>640.49558995927453</v>
       </c>
       <c r="AD33">
-        <v>943.0116782943511</v>
+        <v>1266.418152249259</v>
       </c>
       <c r="AE33">
-        <v>1027.843539311232</v>
-      </c>
-      <c r="AF33">
-        <v>509.0746984757775</v>
-      </c>
-      <c r="AG33">
-        <v>640.49558995927453</v>
-      </c>
-      <c r="AH33">
-        <v>1266.418152249259</v>
-      </c>
-      <c r="AI33">
         <v>2430.7488325133063</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>